<commit_message>
Revisado o fluxo das embalagens retornaveis.
</commit_message>
<xml_diff>
--- a/_extrafiles/SAP_TA2_Responsibles.xlsx
+++ b/_extrafiles/SAP_TA2_Responsibles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FABRICADOS_TA2" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FABRICADOS_TA2!$A$2:$L$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SAP_TA2 COMPRAS'!$A$1:$B$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SAP_TA2 COMPRAS'!$A$1:$D$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="163">
   <si>
     <t>Cliente</t>
   </si>
@@ -485,6 +485,99 @@
   </si>
   <si>
     <t>NADIDINI</t>
+  </si>
+  <si>
+    <t>Returnable Packaging</t>
+  </si>
+  <si>
+    <t>GSCM_026</t>
+  </si>
+  <si>
+    <t>Manta térmica</t>
+  </si>
+  <si>
+    <t>Malha de aço (wire mesh)</t>
+  </si>
+  <si>
+    <t>Catalisadores</t>
+  </si>
+  <si>
+    <t>MP - Aço aluminizado e carbono</t>
+  </si>
+  <si>
+    <t>ICY (Outras Tenneco)</t>
+  </si>
+  <si>
+    <t>Arame de solda</t>
+  </si>
+  <si>
+    <t>Componentes fundidos</t>
+  </si>
+  <si>
+    <t>Abraçadeiras</t>
+  </si>
+  <si>
+    <t>Parafusos, arruelas e porcas</t>
+  </si>
+  <si>
+    <t>Elemento flexível</t>
+  </si>
+  <si>
+    <t>Juntas</t>
+  </si>
+  <si>
+    <t>Plasticos</t>
+  </si>
+  <si>
+    <t>Embalagem retornavel</t>
+  </si>
+  <si>
+    <t>Embalagens e etiquetas</t>
+  </si>
+  <si>
+    <t>Coxins e elementos de borracha</t>
+  </si>
+  <si>
+    <t>Componetes hidroformados</t>
+  </si>
+  <si>
+    <t>Estampados (Importado)</t>
+  </si>
+  <si>
+    <t>Tubo dobrado, estampado, furado (Importado)</t>
+  </si>
+  <si>
+    <t>Português</t>
+  </si>
+  <si>
+    <t>Material absorsivo, fibra de vidro</t>
+  </si>
+  <si>
+    <t>Ganchos, suportes tubular (hangers)</t>
+  </si>
+  <si>
+    <t>MP - Chapas e bobinas em Aço inox</t>
+  </si>
+  <si>
+    <t>Suporte do catalisador (Support Mats)</t>
+  </si>
+  <si>
+    <t>MP - Tubo em inox</t>
+  </si>
+  <si>
+    <t>Tubo dobrado, estampado, furado (Nacional)</t>
+  </si>
+  <si>
+    <t>Estampados (Nacional)</t>
+  </si>
+  <si>
+    <t>Conector do sensor (microfundido)</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>16.05.2023</t>
   </si>
 </sst>
 </file>
@@ -527,7 +620,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,6 +651,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -571,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -592,6 +691,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,317 +1918,544 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.28515625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="9"/>
+      <c r="F2" t="str">
+        <f>"COMPRADOS: "&amp;C2&amp;"&lt;/option&gt;"</f>
+        <v>COMPRADOS: Material absorsivo, fibra de vidro&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="9"/>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F27" si="0">"COMPRADOS: "&amp;C3&amp;"&lt;/option&gt;"</f>
+        <v>COMPRADOS: Ganchos, suportes tubular (hangers)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="9"/>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Manta térmica&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="9"/>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Suporte do catalisador (Support Mats)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="9"/>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Malha de aço (wire mesh)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="9"/>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Catalisadores&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="9"/>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: MP - Chapas e bobinas em Aço inox&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="9"/>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: MP - Aço aluminizado e carbono&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="9"/>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: MP - Tubo em inox&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="9"/>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: ICY (Outras Tenneco)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="9"/>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Arame de solda&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="9"/>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Tubo dobrado, estampado, furado (Nacional)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="9"/>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Estampados (Nacional)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" s="9"/>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Conector do sensor (microfundido)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="9"/>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Componentes fundidos&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="9"/>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Abraçadeiras&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Parafusos, arruelas e porcas&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="9"/>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Elemento flexível&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="9"/>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Juntas&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" s="9"/>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Plasticos&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" s="9"/>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Embalagem retornavel&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Embalagens e etiquetas&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" s="9"/>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Coxins e elementos de borracha&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" s="9"/>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Componetes hidroformados&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Tubo dobrado, estampado, furado (Importado)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPRADOS: Estampados (Importado)&lt;/option&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>120</v>
       </c>
-      <c r="C28"/>
+      <c r="D29"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B26">
-    <sortState ref="A2:L21">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D27"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>